<commit_message>
new samples and updates
</commit_message>
<xml_diff>
--- a/SpreadsheetLightDataGridViewExport/Demo1.xlsx
+++ b/SpreadsheetLightDataGridViewExport/Demo1.xlsx
@@ -40,7 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,13 +48,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -69,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,7 +368,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,7 +386,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -389,5 +403,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>